<commit_message>
修复@error: Max Equation Length错误
</commit_message>
<xml_diff>
--- a/data/result.xlsx
+++ b/data/result.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="213">
   <si>
     <t>项目</t>
   </si>
@@ -376,7 +376,7 @@
     <t>海南铁粉-13_1=[0.0]</t>
   </si>
   <si>
-    <t>高返-13_1=[0.0]</t>
+    <t>高返-13_1=[4.174266]</t>
   </si>
   <si>
     <t>铁泥-13_1=[0.6015498]</t>
@@ -403,7 +403,7 @@
     <t>还原铁粉-13_3=[0.0]</t>
   </si>
   <si>
-    <t>高返-13_3=[0.0]</t>
+    <t>高返-13_3=[4.174266]</t>
   </si>
   <si>
     <t>过筛镍矿-13_3=[0.0]</t>
@@ -442,7 +442,7 @@
     <t>巴西精粉-13_4=[0.0]</t>
   </si>
   <si>
-    <t>高返-13_4=[12.5228]</t>
+    <t>高返-13_4=[3.718342]</t>
   </si>
   <si>
     <t>过筛镍矿-13_4=[0.0]</t>
@@ -460,7 +460,7 @@
     <t>印尼粉-13_4=[0.0]</t>
   </si>
   <si>
-    <t>水洗铁-13_4=[0.0]</t>
+    <t>水洗铁-13_4=[0.5526916]</t>
   </si>
   <si>
     <t>马来西亚-13_4=[0.0]</t>
@@ -475,7 +475,7 @@
     <t>赛尔维亚粉-13_5=[0.0]</t>
   </si>
   <si>
-    <t>高返-13_5=[0.0]</t>
+    <t>高返-13_5=[0.1988863]</t>
   </si>
   <si>
     <t>过筛镍矿-13_5=[0.0]</t>
@@ -496,7 +496,7 @@
     <t>还原铁粉-13_5=[0.0]</t>
   </si>
   <si>
-    <t>水洗铁-13_5=[0.0]</t>
+    <t>水洗铁-13_5=[0.5526916]</t>
   </si>
   <si>
     <t>重力除尘灰-13_5=[0.1142943]</t>
@@ -508,7 +508,7 @@
     <t>赛尔维亚粉-13_12=[0.0]</t>
   </si>
   <si>
-    <t>高返-13_12=[0.0]</t>
+    <t>高返-13_12=[0.2570375]</t>
   </si>
   <si>
     <t>过筛镍矿-13_12=[8.0]</t>
@@ -529,7 +529,7 @@
     <t>还原铁粉-13_12=[0.0]</t>
   </si>
   <si>
-    <t>水洗铁-13_12=[0.0]</t>
+    <t>水洗铁-13_12=[1.456512]</t>
   </si>
   <si>
     <t>重力除尘灰-13_12=[0.1142943]</t>
@@ -553,7 +553,7 @@
     <t>FMG低品澳粉-14-1=[0.0]</t>
   </si>
   <si>
-    <t>氧化铁-14-1=[0.0]</t>
+    <t>氧化铁-14-1=[2.076149]</t>
   </si>
   <si>
     <t>铁泥-14-1=[0.0]</t>
@@ -583,7 +583,7 @@
     <t>FMG低品澳粉-14-3=[0.0]</t>
   </si>
   <si>
-    <t>氧化铁-14-3=[0.0]</t>
+    <t>氧化铁-14-3=[1.312939]</t>
   </si>
   <si>
     <t>铁泥-14-3=[0.0]</t>
@@ -625,10 +625,7 @@
     <t>重力除尘灰-14-4=[0.0]</t>
   </si>
   <si>
-    <t>巴西粗粉-14-4=[11.26373]</t>
-  </si>
-  <si>
-    <t>高品澳粉-14-12=[8.390973]</t>
+    <t>高品澳粉-14-12=[15.0]</t>
   </si>
   <si>
     <t>高返-14-12=[0.0]</t>
@@ -637,7 +634,7 @@
     <t>过筛镍矿-14-12=[0.0]</t>
   </si>
   <si>
-    <t>塞拉利昂粉-14-12=[16.14492]</t>
+    <t>塞拉利昂粉-14-12=[14.84864]</t>
   </si>
   <si>
     <t>FMG低品澳粉-14-12=[40.0]</t>
@@ -1274,7 +1271,7 @@
         <v>500</v>
       </c>
       <c r="N6" s="1">
-        <v>0</v>
+        <v>4.174266</v>
       </c>
       <c r="Q6">
         <v>2</v>
@@ -1643,7 +1640,7 @@
         <v>500</v>
       </c>
       <c r="N15" s="1">
-        <v>0</v>
+        <v>4.174266</v>
       </c>
       <c r="Q15">
         <v>2</v>
@@ -2152,7 +2149,7 @@
         <v>500</v>
       </c>
       <c r="N28" s="1">
-        <v>12.5228</v>
+        <v>3.718342</v>
       </c>
       <c r="Q28">
         <v>2</v>
@@ -2413,7 +2410,7 @@
         <v>300</v>
       </c>
       <c r="N34" s="1">
-        <v>0</v>
+        <v>0.5526915999999999</v>
       </c>
       <c r="T34" t="s">
         <v>148</v>
@@ -2633,7 +2630,7 @@
         <v>500</v>
       </c>
       <c r="N39" s="1">
-        <v>0</v>
+        <v>0.1988863</v>
       </c>
       <c r="Q39">
         <v>2</v>
@@ -2923,7 +2920,7 @@
         <v>300</v>
       </c>
       <c r="N46" s="1">
-        <v>0</v>
+        <v>0.5526915999999999</v>
       </c>
       <c r="T46" t="s">
         <v>160</v>
@@ -3102,7 +3099,7 @@
         <v>500</v>
       </c>
       <c r="N50" s="1">
-        <v>0</v>
+        <v>0.2570375</v>
       </c>
       <c r="Q50">
         <v>2</v>
@@ -3392,7 +3389,7 @@
         <v>300</v>
       </c>
       <c r="N57" s="1">
-        <v>0</v>
+        <v>1.456512</v>
       </c>
       <c r="T57" t="s">
         <v>171</v>
@@ -3750,7 +3747,7 @@
         <v>800</v>
       </c>
       <c r="N65" s="1">
-        <v>0</v>
+        <v>2.076149</v>
       </c>
       <c r="T65" t="s">
         <v>179</v>
@@ -4208,7 +4205,7 @@
         <v>800</v>
       </c>
       <c r="N75" s="1">
-        <v>0</v>
+        <v>1.312939</v>
       </c>
       <c r="T75" t="s">
         <v>189</v>
@@ -4851,10 +4848,10 @@
         <v>566.5</v>
       </c>
       <c r="N89" s="1">
-        <v>11.26373</v>
+        <v>0</v>
       </c>
       <c r="T89" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
     </row>
     <row r="90" spans="1:20">
@@ -4886,7 +4883,7 @@
         <v>600.5</v>
       </c>
       <c r="N90" s="1">
-        <v>8.390973000000001</v>
+        <v>15</v>
       </c>
       <c r="Q90">
         <v>1</v>
@@ -4898,7 +4895,7 @@
         <v>15</v>
       </c>
       <c r="T90" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="91" spans="1:20">
@@ -4948,7 +4945,7 @@
         <v>12.5227971518525</v>
       </c>
       <c r="T91" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="92" spans="1:20">
@@ -4998,7 +4995,7 @@
         <v>15</v>
       </c>
       <c r="T92" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="93" spans="1:20">
@@ -5033,7 +5030,7 @@
         <v>498.015344202792</v>
       </c>
       <c r="N93" s="1">
-        <v>16.14492</v>
+        <v>14.84864</v>
       </c>
       <c r="Q93">
         <v>4</v>
@@ -5045,7 +5042,7 @@
         <v>20</v>
       </c>
       <c r="T93" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="94" spans="1:20">
@@ -5089,7 +5086,7 @@
         <v>40</v>
       </c>
       <c r="T94" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="95" spans="1:20">
@@ -5139,7 +5136,7 @@
         <v>0.60154980513401</v>
       </c>
       <c r="T95" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="96" spans="1:20">
@@ -5189,7 +5186,7 @@
         <v>2.5045594303705</v>
       </c>
       <c r="T96" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="97" spans="1:20">
@@ -5236,7 +5233,7 @@
         <v>0.571471256027976</v>
       </c>
       <c r="T97" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="98" spans="1:20">
@@ -5318,7 +5315,7 @@
         <v>0</v>
       </c>
       <c r="M99" s="1">
-        <v>485.0324705378101</v>
+        <v>489.2533525189781</v>
       </c>
       <c r="N99" s="1" t="s">
         <v>11</v>
@@ -5356,10 +5353,10 @@
         <v>0.18</v>
       </c>
       <c r="M100" s="1">
-        <v>485.0324705378101</v>
+        <v>489.2533525189781</v>
       </c>
       <c r="N100" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="101" spans="1:20">
@@ -5367,10 +5364,10 @@
         <v>99</v>
       </c>
       <c r="M101" s="1">
-        <v>485.0324705378101</v>
+        <v>489.2533525189781</v>
       </c>
       <c r="N101" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="102" spans="1:20" s="1" customFormat="1">
@@ -5381,28 +5378,28 @@
         <v>115</v>
       </c>
       <c r="C102" s="1">
-        <v>55.90000191581774</v>
+        <v>55.90000090477773</v>
       </c>
       <c r="D102" s="1">
-        <v>5.409476629437501</v>
+        <v>4.5000000675375</v>
       </c>
       <c r="E102" s="1">
-        <v>2.33272882205</v>
+        <v>2.897264995189999</v>
       </c>
       <c r="F102" s="1">
-        <v>0.7708580982428573</v>
+        <v>0.9762019118428573</v>
       </c>
       <c r="G102" s="1">
-        <v>3.00000032769</v>
+        <v>3.00000014589</v>
       </c>
       <c r="H102" s="1">
-        <v>0.16553407738</v>
+        <v>0.1632088484</v>
       </c>
       <c r="I102" s="1">
-        <v>0.067777713201</v>
+        <v>0.07965211428500001</v>
       </c>
       <c r="J102" s="1">
-        <v>0.1648</v>
+        <v>0.16721795398</v>
       </c>
     </row>
   </sheetData>

</xml_diff>